<commit_message>
better tile recognition algorithm
</commit_message>
<xml_diff>
--- a/data/game_template.xlsx
+++ b/data/game_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E534E88-11D6-441E-9769-1AEE62DB6F51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBC9341-B3BE-4712-A32F-926B5E16ADE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -702,7 +702,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -782,9 +782,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -824,6 +821,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2226,9 +2229,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>332293</xdr:colOff>
+      <xdr:colOff>326578</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>521856</xdr:rowOff>
+      <xdr:rowOff>514236</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2278,7 +2281,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>134527</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>371381</xdr:rowOff>
+      <xdr:rowOff>365666</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2376,7 +2379,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>42964</xdr:colOff>
+      <xdr:colOff>58204</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>454861</xdr:rowOff>
     </xdr:to>
@@ -2428,7 +2431,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>246053</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>289904</xdr:rowOff>
+      <xdr:rowOff>282284</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2476,9 +2479,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>519029</xdr:colOff>
+      <xdr:colOff>511409</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>310080</xdr:rowOff>
+      <xdr:rowOff>325320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2526,7 +2529,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>69762</xdr:colOff>
+      <xdr:colOff>60237</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>266825</xdr:rowOff>
     </xdr:to>
@@ -2576,9 +2579,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>387298</xdr:colOff>
+      <xdr:colOff>396823</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>444906</xdr:rowOff>
+      <xdr:rowOff>437286</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2726,7 +2729,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>319799</xdr:colOff>
+      <xdr:colOff>327419</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>341322</xdr:rowOff>
     </xdr:to>
@@ -2828,7 +2831,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>532034</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>353674</xdr:rowOff>
+      <xdr:rowOff>359389</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2878,7 +2881,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>320777</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>317346</xdr:rowOff>
+      <xdr:rowOff>324966</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2926,7 +2929,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>300099</xdr:colOff>
+      <xdr:colOff>284859</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>460156</xdr:rowOff>
     </xdr:to>
@@ -2978,7 +2981,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>325810</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>330942</xdr:rowOff>
+      <xdr:rowOff>323322</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3076,9 +3079,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>349538</xdr:colOff>
+      <xdr:colOff>359063</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>336657</xdr:rowOff>
+      <xdr:rowOff>327132</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3228,7 +3231,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>537157</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>386518</xdr:rowOff>
+      <xdr:rowOff>401758</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3278,7 +3281,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>535251</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>373381</xdr:rowOff>
+      <xdr:rowOff>363856</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3378,7 +3381,7 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>98415</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>238585</xdr:rowOff>
+      <xdr:rowOff>244300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3726,477 +3729,487 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9D0752-48DF-4D45-B912-C3CDBBD6BD64}">
   <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="14" width="8.88671875" style="50"/>
+    <col min="1" max="14" width="8.88671875" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="A1" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="E1" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="39" t="s">
+      <c r="A2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="F2" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K3" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3" s="39" t="s">
-        <v>69</v>
-      </c>
+      <c r="A3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="A4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="N5" s="39" t="s">
+      <c r="A5" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="53" t="s">
         <v>67</v>
       </c>
+      <c r="N5" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="L6" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M6" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="39" t="s">
+      <c r="A6" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="53" t="s">
         <v>67</v>
       </c>
+      <c r="N6" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K7" s="39" t="s">
+      <c r="A7" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M7" s="39" t="s">
+      <c r="K7" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="39" t="s">
+      <c r="L7" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="53" t="s">
         <v>67</v>
       </c>
+      <c r="N7" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8" s="39" t="s">
+      <c r="A8" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="L8" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M8" s="39" t="s">
+      <c r="L8" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="N8" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="K9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="N9" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="A9" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="11"/>
       <c r="R9" s="12"/>
-      <c r="S9" s="40" t="s">
+      <c r="S9" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="T9" s="41" t="s">
+      <c r="T9" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="U9" s="42" t="s">
+      <c r="U9" s="41" t="s">
         <v>129</v>
       </c>
       <c r="V9" s="12"/>
     </row>
     <row r="10" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="K10" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="M10" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="N10" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="A10" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="11"/>
       <c r="R10" s="12"/>
-      <c r="S10" s="43">
+      <c r="S10" s="42">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>1</v>
-      </c>
-      <c r="T10" s="44">
+        <v>4</v>
+      </c>
+      <c r="T10" s="43">
         <f t="shared" ref="T10:T11" ca="1" si="0">RANDBETWEEN(1,6)</f>
-        <v>3</v>
-      </c>
-      <c r="U10" s="45">
+        <v>4</v>
+      </c>
+      <c r="U10" s="44">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="V10" s="12"/>
       <c r="W10" t="s">
@@ -4204,207 +4217,211 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="39" t="s">
+      <c r="A11" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="K11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M11" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="N11" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="F11" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="M11" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" s="11"/>
       <c r="R11" s="12"/>
-      <c r="S11" s="43">
+      <c r="S11" s="42">
         <f t="shared" ref="S11:S13" ca="1" si="1">RANDBETWEEN(1,6)</f>
-        <v>1</v>
-      </c>
-      <c r="T11" s="44">
+        <v>4</v>
+      </c>
+      <c r="T11" s="43">
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="U11" s="46"/>
+      <c r="U11" s="45"/>
       <c r="V11" s="12"/>
     </row>
     <row r="12" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="39" t="s">
+      <c r="A12" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="M12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="N12" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="H12" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="M12" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N12" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" s="11"/>
       <c r="R12" s="12"/>
-      <c r="S12" s="43">
+      <c r="S12" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="T12" s="47"/>
-      <c r="U12" s="46"/>
+        <v>6</v>
+      </c>
+      <c r="T12" s="46"/>
+      <c r="U12" s="45"/>
       <c r="V12" s="12"/>
     </row>
     <row r="13" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="39" t="s">
+      <c r="A13" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="L13" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="M13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="N13" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="G13" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="M13" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N13" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O13" s="11"/>
       <c r="R13" s="12"/>
-      <c r="S13" s="48">
+      <c r="S13" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T13" s="18"/>
-      <c r="U13" s="49"/>
+      <c r="U13" s="48"/>
       <c r="V13" s="12"/>
     </row>
     <row r="14" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="L14" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="M14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="N14" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="A14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="M14" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N14" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="O14" s="11"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
@@ -5422,25 +5439,25 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
       <c r="J1" s="12"/>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
@@ -6639,12 +6656,12 @@
       <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="1" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
better UI + watchtowers for combat
</commit_message>
<xml_diff>
--- a/data/game_template.xlsx
+++ b/data/game_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846EBA98-C4EC-465F-AAC3-9565C8B1CA06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B57D0B-DC8F-4B9E-B30D-0960A78D6821}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ui" sheetId="10" r:id="rId1"/>
@@ -442,9 +442,6 @@
     <t>Survivors</t>
   </si>
   <si>
-    <t>3 survivors arrive! You can choose not to take them in and they go to the next player to you, which also has the same choice. If they aren't accepted by anyone they die.</t>
-  </si>
-  <si>
     <t>each wounded survivor consumes 1 to be healed for the next turn. If not enough, the wounded don't heal and one of them dies.</t>
   </si>
   <si>
@@ -497,6 +494,9 @@
   </si>
   <si>
     <t>points</t>
+  </si>
+  <si>
+    <t>3+R survivors arrive! (R=number of radio stations you possess). You can choose not to take them in and they go to the next player to you, which also has the same choice. If they aren't accepted by anyone they die.</t>
   </si>
 </sst>
 </file>
@@ -825,6 +825,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -834,9 +837,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2232,15 +2232,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>95661</xdr:colOff>
+      <xdr:colOff>486186</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>437369</xdr:rowOff>
+      <xdr:rowOff>475469</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>326578</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>107503</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>514236</xdr:rowOff>
+      <xdr:rowOff>552336</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2269,8 +2269,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8630061" y="1008869"/>
-          <a:ext cx="846232" cy="655987"/>
+          <a:off x="8753886" y="1046969"/>
+          <a:ext cx="840517" cy="648367"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2281,16 +2281,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>535607</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>335582</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>198026</xdr:rowOff>
+      <xdr:rowOff>388526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>134527</xdr:colOff>
+      <xdr:colOff>544102</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>365666</xdr:rowOff>
+      <xdr:rowOff>556166</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2319,8 +2319,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9679607" y="1341026"/>
-          <a:ext cx="208520" cy="173355"/>
+          <a:off x="9822482" y="1531526"/>
+          <a:ext cx="208520" cy="167640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2331,16 +2331,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>279149</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2924</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180441</xdr:rowOff>
+      <xdr:rowOff>8991</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>284868</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>8643</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>245211</xdr:rowOff>
+      <xdr:rowOff>73761</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2369,7 +2369,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8813549" y="180441"/>
+          <a:off x="8880224" y="8991"/>
           <a:ext cx="615319" cy="636270"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2382,15 +2382,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>390459</xdr:colOff>
+      <xdr:colOff>57084</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>226261</xdr:rowOff>
+      <xdr:rowOff>188161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>58204</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>334429</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>454861</xdr:rowOff>
+      <xdr:rowOff>416761</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2419,8 +2419,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10753659" y="1369261"/>
-          <a:ext cx="262105" cy="228600"/>
+          <a:off x="10153584" y="1331161"/>
+          <a:ext cx="277345" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2432,15 +2432,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>222171</xdr:colOff>
+      <xdr:colOff>3096</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>227039</xdr:rowOff>
+      <xdr:rowOff>17489</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>246053</xdr:colOff>
+      <xdr:colOff>26978</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>282284</xdr:rowOff>
+      <xdr:rowOff>72734</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2469,8 +2469,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11194971" y="227039"/>
-          <a:ext cx="633482" cy="634365"/>
+          <a:off x="10709196" y="17489"/>
+          <a:ext cx="633482" cy="626745"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2481,16 +2481,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>492968</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>16718</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>245310</xdr:rowOff>
+      <xdr:rowOff>16710</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>511409</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>35159</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>325320</xdr:rowOff>
+      <xdr:rowOff>96720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2519,8 +2519,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9636968" y="245310"/>
-          <a:ext cx="635661" cy="636270"/>
+          <a:off x="9503618" y="16710"/>
+          <a:ext cx="628041" cy="651510"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2532,15 +2532,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>53226</xdr:colOff>
+      <xdr:colOff>15126</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>207770</xdr:rowOff>
+      <xdr:rowOff>26795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>60237</xdr:colOff>
+      <xdr:colOff>22137</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>266825</xdr:rowOff>
+      <xdr:rowOff>85850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2569,8 +2569,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10416426" y="207770"/>
-          <a:ext cx="626136" cy="630555"/>
+          <a:off x="10111626" y="26795"/>
+          <a:ext cx="616611" cy="630555"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2582,15 +2582,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>119975</xdr:colOff>
+      <xdr:colOff>72350</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>172491</xdr:rowOff>
+      <xdr:rowOff>10566</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>396823</xdr:colOff>
+      <xdr:colOff>349198</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>437286</xdr:rowOff>
+      <xdr:rowOff>275361</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2619,8 +2619,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11092775" y="1315491"/>
-          <a:ext cx="267323" cy="272415"/>
+          <a:off x="10778450" y="1153566"/>
+          <a:ext cx="276848" cy="264795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2632,15 +2632,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>412555</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>193955</xdr:rowOff>
+      <xdr:colOff>260155</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>527330</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>134261</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>591461</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>513995</xdr:rowOff>
+      <xdr:rowOff>275870</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2669,7 +2669,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11385355" y="1336955"/>
+          <a:off x="10966255" y="1098830"/>
           <a:ext cx="331306" cy="320040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2682,15 +2682,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>220668</xdr:colOff>
+      <xdr:colOff>11118</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>167982</xdr:rowOff>
+      <xdr:rowOff>329907</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>570586</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>436587</xdr:rowOff>
+      <xdr:colOff>361036</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>27012</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2719,7 +2719,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9974268" y="1310982"/>
+          <a:off x="9498018" y="1472907"/>
           <a:ext cx="349918" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2782,15 +2782,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>369311</xdr:colOff>
+      <xdr:colOff>426461</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>217630</xdr:rowOff>
+      <xdr:rowOff>8080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>551740</xdr:colOff>
+      <xdr:colOff>608890</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>400510</xdr:rowOff>
+      <xdr:rowOff>190960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2819,7 +2819,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9513311" y="2503630"/>
+          <a:off x="9303761" y="2294080"/>
           <a:ext cx="182429" cy="182880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2832,15 +2832,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>355320</xdr:colOff>
+      <xdr:colOff>431520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>176509</xdr:rowOff>
+      <xdr:rowOff>5059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>532034</xdr:colOff>
+      <xdr:colOff>608234</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>359389</xdr:rowOff>
+      <xdr:rowOff>187939</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2869,8 +2869,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9499320" y="1891009"/>
-          <a:ext cx="176714" cy="177165"/>
+          <a:off x="9308820" y="1719559"/>
+          <a:ext cx="176714" cy="182880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2932,15 +2932,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>32845</xdr:colOff>
+      <xdr:colOff>280495</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>183931</xdr:rowOff>
+      <xdr:rowOff>164881</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>284859</xdr:colOff>
+      <xdr:colOff>532509</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>460156</xdr:rowOff>
+      <xdr:rowOff>441106</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2969,8 +2969,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10396045" y="1326931"/>
-          <a:ext cx="267254" cy="276225"/>
+          <a:off x="10376995" y="1307881"/>
+          <a:ext cx="252014" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3182,15 +3182,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>353413</xdr:colOff>
+      <xdr:colOff>429613</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>203637</xdr:rowOff>
+      <xdr:rowOff>32187</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>535251</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1851</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>384612</xdr:rowOff>
+      <xdr:rowOff>213162</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3219,7 +3219,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9497413" y="3061137"/>
+          <a:off x="9306913" y="2889687"/>
           <a:ext cx="181838" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3232,15 +3232,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>357224</xdr:colOff>
+      <xdr:colOff>433424</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>207448</xdr:rowOff>
+      <xdr:rowOff>35998</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>537157</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>3757</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>401758</xdr:rowOff>
+      <xdr:rowOff>230308</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3269,8 +3269,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9501224" y="3636448"/>
-          <a:ext cx="179933" cy="179070"/>
+          <a:off x="9310724" y="3464998"/>
+          <a:ext cx="179933" cy="194310"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3282,15 +3282,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>347698</xdr:colOff>
+      <xdr:colOff>423898</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>186691</xdr:rowOff>
+      <xdr:rowOff>15241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>535251</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1851</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>363856</xdr:rowOff>
+      <xdr:rowOff>192406</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3319,8 +3319,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9491698" y="4187191"/>
-          <a:ext cx="187553" cy="186690"/>
+          <a:off x="9301198" y="4015741"/>
+          <a:ext cx="187553" cy="177165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3332,15 +3332,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>362741</xdr:colOff>
+      <xdr:colOff>438941</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>185836</xdr:rowOff>
+      <xdr:rowOff>14386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>550885</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>17485</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>364906</xdr:rowOff>
+      <xdr:rowOff>193456</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3369,7 +3369,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9506741" y="4757836"/>
+          <a:off x="9316241" y="4586386"/>
           <a:ext cx="188144" cy="179070"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3382,15 +3382,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>362607</xdr:colOff>
+      <xdr:colOff>153057</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>262759</xdr:rowOff>
+      <xdr:rowOff>5584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>98415</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>244300</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>498465</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>558625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3419,8 +3419,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11945007" y="262759"/>
-          <a:ext cx="345408" cy="547326"/>
+          <a:off x="11468757" y="5584"/>
+          <a:ext cx="345408" cy="553041"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3738,16 +3738,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9D0752-48DF-4D45-B912-C3CDBBD6BD64}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="8.88671875" style="49"/>
+    <col min="1" max="14" width="8.85546875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>68</v>
       </c>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>68</v>
       </c>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="O2" s="11"/>
     </row>
-    <row r="3" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>69</v>
       </c>
@@ -3882,7 +3882,7 @@
       </c>
       <c r="O3" s="11"/>
     </row>
-    <row r="4" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>69</v>
       </c>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="O4" s="11"/>
     </row>
-    <row r="5" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
         <v>68</v>
       </c>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="O5" s="11"/>
     </row>
-    <row r="6" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
         <v>68</v>
       </c>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="O6" s="11"/>
     </row>
-    <row r="7" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
         <v>68</v>
       </c>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="O7" s="11"/>
     </row>
-    <row r="8" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>68</v>
       </c>
@@ -4107,7 +4107,7 @@
       </c>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>68</v>
       </c>
@@ -4154,7 +4154,7 @@
       <c r="R9" s="12"/>
       <c r="V9" s="12"/>
     </row>
-    <row r="10" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>68</v>
       </c>
@@ -4199,17 +4199,17 @@
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q10" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="Q10" s="40" t="s">
+      <c r="R10" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="R10" s="41" t="s">
-        <v>129</v>
-      </c>
       <c r="V10" s="12"/>
     </row>
-    <row r="11" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="50" t="s">
         <v>68</v>
       </c>
@@ -4255,19 +4255,19 @@
       <c r="O11" s="11"/>
       <c r="P11" s="42">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="43">
         <f t="shared" ref="Q11:Q12" ca="1" si="0">RANDBETWEEN(1,6)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R11" s="44">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V11" s="12"/>
     </row>
-    <row r="12" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50" t="s">
         <v>68</v>
       </c>
@@ -4313,16 +4313,16 @@
       <c r="O12" s="11"/>
       <c r="P12" s="42">
         <f t="shared" ref="P12:P14" ca="1" si="1">RANDBETWEEN(1,6)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="R12" s="45"/>
       <c r="V12" s="12"/>
     </row>
-    <row r="13" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="50" t="s">
         <v>68</v>
       </c>
@@ -4368,13 +4368,13 @@
       <c r="O13" s="11"/>
       <c r="P13" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q13" s="46"/>
       <c r="R13" s="45"/>
       <c r="V13" s="12"/>
     </row>
-    <row r="14" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="s">
         <v>68</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="O14" s="11"/>
       <c r="P14" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="18"/>
       <c r="R14" s="48"/>
@@ -4429,56 +4429,56 @@
       <c r="U14" s="12"/>
       <c r="V14" s="12"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="55" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="57" t="s">
+      <c r="B15" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="56" t="s">
+      <c r="G15" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="56" t="s">
+      <c r="I15" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="56" t="s">
+      <c r="K15" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="55" t="s">
+      <c r="L15" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="M15" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="M15" s="57" t="s">
+      <c r="N15" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="N15" s="57" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>1</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="13">
         <v>3</v>
@@ -4517,12 +4517,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>2</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="13">
         <v>3</v>
@@ -4561,12 +4561,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>3</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="13">
         <v>3</v>
@@ -4605,12 +4605,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>4</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="13">
         <v>3</v>
@@ -4649,12 +4649,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>5</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="48">
         <v>3</v>
@@ -4707,12 +4707,12 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="15" width="5.77734375" customWidth="1"/>
+    <col min="4" max="15" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="U1" s="31"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>3</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>4</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>5</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>6</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>7</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>8</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>9</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>10</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
@@ -5188,7 +5188,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="16"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>31</v>
       </c>
@@ -5311,15 +5311,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="32.77734375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="32.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>33</v>
@@ -5339,7 +5339,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -5373,11 +5373,11 @@
         <v>24</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>79</v>
@@ -5397,7 +5397,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5411,11 +5411,11 @@
         <v>23</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5429,11 +5429,11 @@
         <v>23</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5506,30 +5506,30 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D1" s="52" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D1" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
       <c r="J1" s="12"/>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-    </row>
-    <row r="2" spans="1:21" s="8" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+    </row>
+    <row r="2" spans="1:21" s="8" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5622,7 +5622,7 @@
       <c r="Q3" s="12"/>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5658,7 +5658,7 @@
       <c r="Q4" s="12"/>
       <c r="R4" s="13"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5858,7 +5858,7 @@
       <c r="Q9" s="12"/>
       <c r="R9" s="13"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5891,7 +5891,7 @@
       <c r="Q10" s="12"/>
       <c r="R10" s="13"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5922,7 +5922,7 @@
       <c r="Q11" s="12"/>
       <c r="R11" s="13"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5953,7 +5953,7 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="13"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -5970,7 +5970,7 @@
       <c r="Q13" s="12"/>
       <c r="R13" s="13"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -5987,7 +5987,7 @@
       <c r="Q14" s="12"/>
       <c r="R14" s="13"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -6004,7 +6004,7 @@
       <c r="Q15" s="12"/>
       <c r="R15" s="13"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -6021,7 +6021,7 @@
       <c r="Q16" s="12"/>
       <c r="R16" s="13"/>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -6038,7 +6038,7 @@
       <c r="Q17" s="12"/>
       <c r="R17" s="13"/>
     </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -6055,7 +6055,7 @@
       <c r="Q18" s="12"/>
       <c r="R18" s="13"/>
     </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -6072,7 +6072,7 @@
       <c r="Q19" s="12"/>
       <c r="R19" s="13"/>
     </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -6107,9 +6107,9 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="34">
         <v>1</v>
       </c>
@@ -6141,10 +6141,10 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="34">
         <v>2</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <v>3</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="34">
         <v>4</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
         <v>5</v>
       </c>
@@ -6213,10 +6213,10 @@
         <v>0.2</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
         <v>6</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" s="32"/>
     </row>
   </sheetData>
@@ -6246,13 +6246,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE295004-92D0-4869-98E3-E69FBF91F6CE}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="34">
         <v>1</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>You find WATER! You get 15+10S, where S is the number of scavengers, if you have at least one active scavenger</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="34">
         <v>2</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>You find FOOD! You get 15+10S, where S is the number of scavengers, if you have at least one active scavenger</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <v>3</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>You find MEDICINES! You get 5+3S, where S is the number of scavengers, if you have at least one active scavenger</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="34">
         <v>4</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>You find ROCK! You get 5+3S, where S is the number of scavengers, if you have at least one active scavenger</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
         <v>5</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>You find WOOD! You get 5+3S, where S is the number of scavengers, if you have at least one active scavenger</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
         <v>6</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>You find TOOLS! You get 5+3S, where S is the number of scavengers, if you have at least one active scavenger</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
         <v>7</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>You find WEAPONS! You get 5+3S, where S is the number of scavengers, if you have at least one active scavenger</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="34">
         <v>8</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>You find INFORMATION! You get 5+3S, where S is the number of scavengers, if you have at least one active scavenger</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <v>9</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <v>10</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <v>11</v>
       </c>
@@ -6472,10 +6472,10 @@
         <v>0.13761467889908258</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="34">
         <v>12</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>13</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>You found a WELL! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="34">
         <v>14</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>You found a WATER CLEANER! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <v>15</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>You found a FARMACY! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="34">
         <v>16</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>You found a WORKSHOP! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>17</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>You found a RADIO STATION! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="34">
         <v>18</v>
       </c>
@@ -6608,7 +6608,7 @@
       </c>
       <c r="P19" s="33"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <v>19</v>
       </c>
@@ -6627,7 +6627,7 @@
         <v>You found a FARM! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="34">
         <v>20</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>You found a HUNTER CAMP! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="34">
         <v>21</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>You found a LUMBER CAMP! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="34">
         <v>22</v>
       </c>
@@ -6684,11 +6684,11 @@
         <v>You found a QUARRY! Place it in whichever building (not necessarily yours) or tile you want</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="34"/>
       <c r="D24" s="33"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="D25" s="33"/>
     </row>
@@ -6705,9 +6705,9 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -6726,17 +6726,17 @@
       <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
       <c r="K1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="34">
         <v>1</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="34">
         <v>2</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <v>3</v>
       </c>
@@ -6836,7 +6836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="34">
         <v>4</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
         <v>5</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
         <v>6</v>
       </c>
@@ -6923,7 +6923,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
         <v>7</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="34">
         <v>8</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <v>9</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <v>10</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <v>11</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="34">
         <v>12</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>13</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="34">
         <v>14</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <v>15</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="34">
         <v>16</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>17</v>
       </c>
@@ -7249,7 +7249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="34">
         <v>18</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <v>19</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="34">
         <v>20</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="34">
         <v>21</v>
       </c>
@@ -7361,7 +7361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="34">
         <v>22</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="34">
         <v>23</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="34">
         <v>24</v>
       </c>
@@ -7445,7 +7445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="34">
         <v>25</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
     </row>
   </sheetData>

</xml_diff>